<commit_message>
Added version and update date to the Excel
</commit_message>
<xml_diff>
--- a/Data/source.xlsx
+++ b/Data/source.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,37 +50,62 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -92,7 +121,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -457,42 +486,50 @@
   </sheetPr>
   <dimension ref="A1:Y1170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-    <col width="15" customWidth="1" min="11" max="11"/>
-    <col width="15" customWidth="1" min="12" max="12"/>
-    <col width="15" customWidth="1" min="13" max="13"/>
-    <col width="15" customWidth="1" min="14" max="14"/>
-    <col width="15" customWidth="1" min="15" max="15"/>
-    <col width="15" customWidth="1" min="16" max="16"/>
-    <col width="15" customWidth="1" min="17" max="17"/>
-    <col width="15" customWidth="1" min="18" max="18"/>
-    <col width="15" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
-    <col width="15" customWidth="1" min="21" max="21"/>
-    <col width="15" customWidth="1" min="22" max="22"/>
-    <col width="15" customWidth="1" min="23" max="23"/>
-    <col width="15" customWidth="1" min="24" max="24"/>
-    <col width="15" customWidth="1" min="25" max="25"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="18" customWidth="1" min="12" max="12"/>
+    <col width="18" customWidth="1" min="13" max="13"/>
+    <col width="18" customWidth="1" min="14" max="14"/>
+    <col width="18" customWidth="1" min="15" max="15"/>
+    <col width="18" customWidth="1" min="16" max="16"/>
+    <col width="18" customWidth="1" min="17" max="17"/>
+    <col width="18" customWidth="1" min="18" max="18"/>
+    <col width="18" customWidth="1" min="19" max="19"/>
+    <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="18" customWidth="1" min="21" max="21"/>
+    <col width="18" customWidth="1" min="22" max="22"/>
+    <col width="18" customWidth="1" min="23" max="23"/>
+    <col width="18" customWidth="1" min="24" max="24"/>
+    <col width="18" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Güncelleme zamanı</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>18.11.2022  09:20</t>
+        </is>
+      </c>
       <c r="C1" s="2" t="n"/>
       <c r="D1" s="3" t="n"/>
       <c r="E1" s="1" t="inlineStr">
@@ -546,7 +583,11 @@
       <c r="Y1" s="3" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr"/>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Versiyon - 00</t>
+        </is>
+      </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
           <t>Cihaz TTNr</t>
@@ -26794,6 +26835,6 @@
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added color formatting and headers
</commit_message>
<xml_diff>
--- a/Data/source.xlsx
+++ b/Data/source.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,13 +32,24 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -112,9 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -520,72 +534,72 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Güncelleme zamanı</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>18.11.2022  09:20</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="3" t="n"/>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Versiyon - 00</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Güncelleme zamanı:  18.11.2022  09:20</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="4" t="n"/>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Pazartesi - 21 Nov 2022</t>
         </is>
       </c>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="3" t="n"/>
+      <c r="F1" s="3" t="n"/>
+      <c r="G1" s="4" t="n"/>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Salı - 22 Nov 2022</t>
         </is>
       </c>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="3" t="n"/>
+      <c r="I1" s="3" t="n"/>
+      <c r="J1" s="4" t="n"/>
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Çarşamba - 23 Nov 2022</t>
         </is>
       </c>
-      <c r="L1" s="2" t="n"/>
-      <c r="M1" s="3" t="n"/>
+      <c r="L1" s="3" t="n"/>
+      <c r="M1" s="4" t="n"/>
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Perşembe - 24 Nov 2022</t>
         </is>
       </c>
-      <c r="O1" s="2" t="n"/>
-      <c r="P1" s="3" t="n"/>
+      <c r="O1" s="3" t="n"/>
+      <c r="P1" s="4" t="n"/>
       <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Cuma - 25 Nov 2022</t>
         </is>
       </c>
-      <c r="R1" s="2" t="n"/>
-      <c r="S1" s="3" t="n"/>
+      <c r="R1" s="3" t="n"/>
+      <c r="S1" s="4" t="n"/>
       <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Cumartesi - 26 Nov 2022</t>
         </is>
       </c>
-      <c r="U1" s="2" t="n"/>
-      <c r="V1" s="3" t="n"/>
+      <c r="U1" s="3" t="n"/>
+      <c r="V1" s="4" t="n"/>
       <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Pazar - 27 Nov 2022</t>
         </is>
       </c>
-      <c r="X1" s="2" t="n"/>
-      <c r="Y1" s="3" t="n"/>
+      <c r="X1" s="3" t="n"/>
+      <c r="Y1" s="4" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Versiyon - 00</t>
+          <t>Hat</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Added file configuration settings
</commit_message>
<xml_diff>
--- a/Data/source.xlsx
+++ b/Data/source.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -27,12 +28,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -63,62 +59,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -152,7 +123,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -517,7 +488,7 @@
   </sheetPr>
   <dimension ref="A1:Y1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -49684,6 +49655,6 @@
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>